<commit_message>
Updating to reflect article revisions
</commit_message>
<xml_diff>
--- a/Sample Groupings and Ground Truth Labels.xlsx
+++ b/Sample Groupings and Ground Truth Labels.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="17">
   <si>
     <t>Patient ID</t>
   </si>
@@ -34,16 +34,19 @@
     <t>MRI Scanner Model</t>
   </si>
   <si>
-    <t>Renal</t>
+    <t>Lung</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Melanoma</t>
+    <t>Breast</t>
   </si>
   <si>
-    <t>Breast</t>
+    <t>Renal</t>
+  </si>
+  <si>
+    <t>Skin</t>
   </si>
   <si>
     <t>Colorectal</t>
@@ -82,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -102,27 +105,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -136,22 +123,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,28 +138,28 @@
     <col min="1" max="1" width="3.140625" customWidth="true"/>
     <col min="2" max="2" width="2.140625" customWidth="true"/>
     <col min="3" max="3" width="2.140625" customWidth="true"/>
-    <col min="4" max="4" width="18.28515625" customWidth="true"/>
+    <col min="4" max="4" width="10.140625" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
     <col min="6" max="6" width="24.85546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -202,14 +173,14 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E2">
         <v>0.089999999999999997</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>11</v>
+      <c r="F2" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -222,14 +193,14 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3">
         <v>0.043000000000000003</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>11</v>
+      <c r="F3" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -242,14 +213,14 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4">
         <v>26.098830754303734</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>12</v>
+      <c r="F4" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -262,14 +233,14 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E5">
         <v>0.86024553283186966</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>12</v>
+      <c r="F5" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -282,14 +253,14 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E6">
         <v>0.88800000000000001</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>13</v>
+      <c r="F6" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -302,14 +273,14 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E7">
         <v>0.92390294117647542</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>11</v>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -322,14 +293,14 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E8">
         <v>0.19966764705882459</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>11</v>
+      <c r="F8" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -342,14 +313,14 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E9">
         <v>1.1260000000000001</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>11</v>
+      <c r="F9" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -362,14 +333,14 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E10">
         <v>1.6651153564453125</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>14</v>
+      <c r="F10" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -382,14 +353,14 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E11">
         <v>2.655029296875</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>14</v>
+      <c r="F11" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -402,14 +373,14 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E12">
         <v>9.3454999999999995</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>11</v>
+      <c r="F12" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -422,14 +393,14 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E13">
         <v>3.4485000000000001</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>11</v>
+      <c r="F13" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -442,14 +413,14 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E14">
         <v>6.6361427307128906</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>14</v>
+      <c r="F14" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15">
@@ -462,14 +433,14 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E15">
         <v>3.2601356506347656</v>
       </c>
-      <c r="F15" s="21" t="s">
-        <v>14</v>
+      <c r="F15" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -482,14 +453,14 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>7</v>
+      <c r="D16" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E16">
         <v>7.814368549063186</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>12</v>
+      <c r="F16" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -502,14 +473,14 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E17">
         <v>2.22015380859375</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>14</v>
+      <c r="F17" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -522,14 +493,14 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E18">
         <v>6.5603256225585938</v>
       </c>
-      <c r="F18" s="21" t="s">
-        <v>14</v>
+      <c r="F18" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19">
@@ -542,14 +513,14 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E19">
         <v>12.97325</v>
       </c>
-      <c r="F19" s="21" t="s">
-        <v>11</v>
+      <c r="F19" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -562,14 +533,14 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E20">
         <v>0.23725000000000002</v>
       </c>
-      <c r="F20" s="21" t="s">
-        <v>11</v>
+      <c r="F20" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -582,14 +553,14 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E21">
         <v>3.50189208984375</v>
       </c>
-      <c r="F21" s="21" t="s">
-        <v>14</v>
+      <c r="F21" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -602,14 +573,14 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E22">
         <v>3.54</v>
       </c>
-      <c r="F22" s="21" t="s">
-        <v>13</v>
+      <c r="F22" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -622,14 +593,14 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>7</v>
+      <c r="D23" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E23">
         <v>1.7615225137757857</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>12</v>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24">
@@ -642,14 +613,14 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>10</v>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E24">
         <v>7.6684999999999999</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>11</v>
+      <c r="F24" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25">
@@ -662,14 +633,14 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E25">
         <v>5.9489999999999998</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>11</v>
+      <c r="F25" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26">
@@ -682,14 +653,14 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>10</v>
+      <c r="D26" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E26">
         <v>30.226707458496094</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>14</v>
+      <c r="F26" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27">
@@ -702,14 +673,14 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E27">
         <v>9.6120000000000001</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>13</v>
+      <c r="F27" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28">
@@ -722,14 +693,14 @@
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E28">
         <v>1.9783973693847656</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>14</v>
+      <c r="F28" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -742,14 +713,14 @@
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E29">
         <v>4.62425</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>11</v>
+      <c r="F29" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30">
@@ -762,14 +733,14 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E30">
         <v>9.7258680800761059</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>12</v>
+      <c r="F30" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31">
@@ -782,14 +753,14 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>7</v>
+      <c r="D31" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E31">
         <v>3.0356872558593753</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>14</v>
+      <c r="F31" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -802,14 +773,14 @@
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E32">
         <v>0.8248735948042436</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>12</v>
+      <c r="F32" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33">
@@ -822,14 +793,14 @@
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E33">
         <v>3.5290718078613281</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>14</v>
+      <c r="F33" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34">
@@ -842,14 +813,14 @@
       <c r="C34">
         <v>0</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E34">
         <v>2.7650000000000001</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>11</v>
+      <c r="F34" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="35">
@@ -862,14 +833,14 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E35">
         <v>3.4475326538085938</v>
       </c>
-      <c r="F35" s="21" t="s">
-        <v>14</v>
+      <c r="F35" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -882,14 +853,14 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E36">
         <v>28.103712201709591</v>
       </c>
-      <c r="F36" s="21" t="s">
-        <v>12</v>
+      <c r="F36" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37">
@@ -902,14 +873,14 @@
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E37">
         <v>6.7930000000000001</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>11</v>
+      <c r="F37" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38">
@@ -922,14 +893,14 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E38">
         <v>15.752999999999664</v>
       </c>
-      <c r="F38" s="21" t="s">
-        <v>11</v>
+      <c r="F38" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -942,14 +913,14 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E39">
         <v>5.4373741149902344</v>
       </c>
-      <c r="F39" s="21" t="s">
-        <v>14</v>
+      <c r="F39" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40">
@@ -962,14 +933,14 @@
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E40">
         <v>11.750557812777432</v>
       </c>
-      <c r="F40" s="21" t="s">
-        <v>12</v>
+      <c r="F40" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41">
@@ -982,14 +953,14 @@
       <c r="C41">
         <v>0</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E41">
         <v>18.234729766845703</v>
       </c>
-      <c r="F41" s="21" t="s">
-        <v>14</v>
+      <c r="F41" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="42">
@@ -1002,14 +973,14 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E42">
         <v>4.4102668762207031</v>
       </c>
-      <c r="F42" s="21" t="s">
-        <v>14</v>
+      <c r="F42" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="43">
@@ -1022,14 +993,14 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E43">
         <v>1.3427187675286916</v>
       </c>
-      <c r="F43" s="21" t="s">
-        <v>12</v>
+      <c r="F43" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44">
@@ -1042,14 +1013,14 @@
       <c r="C44">
         <v>0</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E44">
         <v>16.197220588235709</v>
       </c>
-      <c r="F44" s="21" t="s">
-        <v>11</v>
+      <c r="F44" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="45">
@@ -1062,14 +1033,14 @@
       <c r="C45">
         <v>0</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E45">
         <v>1.491723529411803</v>
       </c>
-      <c r="F45" s="21" t="s">
-        <v>11</v>
+      <c r="F45" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="46">
@@ -1082,14 +1053,14 @@
       <c r="C46">
         <v>0</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E46">
         <v>4.1556358337402344</v>
       </c>
-      <c r="F46" s="21" t="s">
-        <v>14</v>
+      <c r="F46" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47">
@@ -1102,14 +1073,14 @@
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E47">
         <v>0.018596649169921875</v>
       </c>
-      <c r="F47" s="21" t="s">
-        <v>14</v>
+      <c r="F47" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="48">
@@ -1122,14 +1093,14 @@
       <c r="C48">
         <v>0</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>7</v>
+      <c r="D48" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E48">
         <v>1.0555000000000001</v>
       </c>
-      <c r="F48" s="21" t="s">
-        <v>11</v>
+      <c r="F48" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49">
@@ -1142,14 +1113,14 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49" s="17" t="s">
-        <v>7</v>
+      <c r="D49" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E49">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F49" s="21" t="s">
-        <v>11</v>
+      <c r="F49" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50">
@@ -1162,14 +1133,14 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>7</v>
+      <c r="D50" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E50">
         <v>2.7038309428317491</v>
       </c>
-      <c r="F50" s="21" t="s">
-        <v>12</v>
+      <c r="F50" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51">
@@ -1182,14 +1153,14 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E51">
         <v>16.491812386000454</v>
       </c>
-      <c r="F51" s="21" t="s">
-        <v>12</v>
+      <c r="F51" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52">
@@ -1202,14 +1173,14 @@
       <c r="C52">
         <v>0</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E52">
         <v>2.2256023406982424</v>
       </c>
-      <c r="F52" s="21" t="s">
-        <v>12</v>
+      <c r="F52" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53">
@@ -1222,14 +1193,14 @@
       <c r="C53">
         <v>0</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53">
         <v>0.80506553374046141</v>
       </c>
-      <c r="F53" s="21" t="s">
-        <v>12</v>
+      <c r="F53" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="54">
@@ -1242,14 +1213,14 @@
       <c r="C54">
         <v>0</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54">
         <v>0.13582827985779314</v>
       </c>
-      <c r="F54" s="21" t="s">
-        <v>12</v>
+      <c r="F54" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55">
@@ -1262,14 +1233,14 @@
       <c r="C55">
         <v>0</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55">
         <v>3.8785000000000003</v>
       </c>
-      <c r="F55" s="21" t="s">
-        <v>11</v>
+      <c r="F55" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="56">
@@ -1282,14 +1253,14 @@
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E56">
         <v>4.2658557261317229</v>
       </c>
-      <c r="F56" s="21" t="s">
-        <v>12</v>
+      <c r="F56" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57">
@@ -1302,14 +1273,14 @@
       <c r="C57">
         <v>0</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E57">
         <v>0.29004989182653501</v>
       </c>
-      <c r="F57" s="21" t="s">
-        <v>12</v>
+      <c r="F57" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="58">
@@ -1322,14 +1293,14 @@
       <c r="C58">
         <v>0</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E58">
         <v>0.01556365273215554</v>
       </c>
-      <c r="F58" s="21" t="s">
-        <v>12</v>
+      <c r="F58" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="59">
@@ -1342,14 +1313,14 @@
       <c r="C59">
         <v>0</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E59">
         <v>3.1092499999999998</v>
       </c>
-      <c r="F59" s="21" t="s">
-        <v>11</v>
+      <c r="F59" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60">
@@ -1362,14 +1333,14 @@
       <c r="C60">
         <v>0</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E60">
         <v>1.0825</v>
       </c>
-      <c r="F60" s="21" t="s">
-        <v>11</v>
+      <c r="F60" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="61">
@@ -1382,14 +1353,14 @@
       <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61" s="17" t="s">
-        <v>10</v>
+      <c r="D61" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E61">
         <v>20.197749999999999</v>
       </c>
-      <c r="F61" s="21" t="s">
-        <v>11</v>
+      <c r="F61" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62">
@@ -1402,14 +1373,14 @@
       <c r="C62">
         <v>0</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E62">
         <v>2.1187499999999999</v>
       </c>
-      <c r="F62" s="21" t="s">
-        <v>11</v>
+      <c r="F62" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="63">
@@ -1422,14 +1393,14 @@
       <c r="C63">
         <v>0</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E63">
         <v>0.192</v>
       </c>
-      <c r="F63" s="21" t="s">
-        <v>11</v>
+      <c r="F63" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="64">
@@ -1442,14 +1413,14 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E64">
         <v>0.59775</v>
       </c>
-      <c r="F64" s="21" t="s">
-        <v>11</v>
+      <c r="F64" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="65">
@@ -1462,14 +1433,14 @@
       <c r="C65">
         <v>0</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65">
         <v>7.8864097595214844</v>
       </c>
-      <c r="F65" s="21" t="s">
-        <v>14</v>
+      <c r="F65" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="66">
@@ -1482,14 +1453,14 @@
       <c r="C66">
         <v>0</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E66">
         <v>0.73957443237304688</v>
       </c>
-      <c r="F66" s="21" t="s">
-        <v>14</v>
+      <c r="F66" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -1502,14 +1473,14 @@
       <c r="C67">
         <v>0</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="D67" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E67">
         <v>0.044345855712890625</v>
       </c>
-      <c r="F67" s="21" t="s">
-        <v>14</v>
+      <c r="F67" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="68">
@@ -1522,14 +1493,14 @@
       <c r="C68">
         <v>0</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D68" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E68">
         <v>0.4385</v>
       </c>
-      <c r="F68" s="21" t="s">
-        <v>11</v>
+      <c r="F68" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="69">
@@ -1542,14 +1513,14 @@
       <c r="C69">
         <v>0</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D69" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E69">
         <v>0.26124999999999998</v>
       </c>
-      <c r="F69" s="21" t="s">
-        <v>11</v>
+      <c r="F69" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="70">
@@ -1562,14 +1533,14 @@
       <c r="C70">
         <v>0</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="D70" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E70">
         <v>1.5506744384765625</v>
       </c>
-      <c r="F70" s="21" t="s">
-        <v>14</v>
+      <c r="F70" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="71">
@@ -1582,14 +1553,14 @@
       <c r="C71">
         <v>0</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D71" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E71">
         <v>0.5092620849609375</v>
       </c>
-      <c r="F71" s="21" t="s">
-        <v>12</v>
+      <c r="F71" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="72">
@@ -1602,14 +1573,14 @@
       <c r="C72">
         <v>0</v>
       </c>
-      <c r="D72" s="17" t="s">
-        <v>10</v>
+      <c r="D72" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E72">
         <v>12.4725</v>
       </c>
-      <c r="F72" s="21" t="s">
-        <v>11</v>
+      <c r="F72" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="73">
@@ -1622,14 +1593,14 @@
       <c r="C73">
         <v>0</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D73" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E73">
         <v>11.685848236083984</v>
       </c>
-      <c r="F73" s="21" t="s">
-        <v>14</v>
+      <c r="F73" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="74">
@@ -1642,14 +1613,14 @@
       <c r="C74">
         <v>0</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D74" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E74">
         <v>0.2460479736328125</v>
       </c>
-      <c r="F74" s="21" t="s">
-        <v>14</v>
+      <c r="F74" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="75">
@@ -1662,14 +1633,14 @@
       <c r="C75">
         <v>0</v>
       </c>
-      <c r="D75" s="17" t="s">
-        <v>10</v>
+      <c r="D75" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E75">
         <v>0.148773193359375</v>
       </c>
-      <c r="F75" s="21" t="s">
-        <v>14</v>
+      <c r="F75" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="76">
@@ -1682,14 +1653,14 @@
       <c r="C76">
         <v>1</v>
       </c>
-      <c r="D76" s="17" t="s">
-        <v>10</v>
+      <c r="D76" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E76">
         <v>17.453929100351882</v>
       </c>
-      <c r="F76" s="21" t="s">
-        <v>12</v>
+      <c r="F76" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="77">
@@ -1702,14 +1673,14 @@
       <c r="C77">
         <v>0</v>
       </c>
-      <c r="D77" s="17" t="s">
-        <v>10</v>
+      <c r="D77" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E77">
         <v>0.060839733407517103</v>
       </c>
-      <c r="F77" s="21" t="s">
-        <v>12</v>
+      <c r="F77" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="78">
@@ -1722,14 +1693,14 @@
       <c r="C78">
         <v>0</v>
       </c>
-      <c r="D78" s="17" t="s">
-        <v>10</v>
+      <c r="D78" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E78">
         <v>0.038201693069836319</v>
       </c>
-      <c r="F78" s="21" t="s">
-        <v>12</v>
+      <c r="F78" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="79">
@@ -1742,14 +1713,14 @@
       <c r="C79">
         <v>0</v>
       </c>
-      <c r="D79" s="17" t="s">
+      <c r="D79" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E79">
         <v>5.4159164428710938</v>
       </c>
-      <c r="F79" s="21" t="s">
-        <v>12</v>
+      <c r="F79" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="80">
@@ -1762,14 +1733,14 @@
       <c r="C80">
         <v>0</v>
       </c>
-      <c r="D80" s="17" t="s">
+      <c r="D80" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E80">
         <v>3.3788681030273438</v>
       </c>
-      <c r="F80" s="21" t="s">
-        <v>14</v>
+      <c r="F80" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="81">
@@ -1782,14 +1753,14 @@
       <c r="C81">
         <v>0</v>
       </c>
-      <c r="D81" s="17" t="s">
+      <c r="D81" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E81">
         <v>0.12874603271484375</v>
       </c>
-      <c r="F81" s="21" t="s">
-        <v>14</v>
+      <c r="F81" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="82">
@@ -1802,14 +1773,14 @@
       <c r="C82">
         <v>0</v>
       </c>
-      <c r="D82" s="17" t="s">
+      <c r="D82" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E82">
         <v>7.5794999999999169</v>
       </c>
-      <c r="F82" s="21" t="s">
-        <v>11</v>
+      <c r="F82" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="83">
@@ -1822,14 +1793,14 @@
       <c r="C83">
         <v>0</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E83">
         <v>1.4804999999999837</v>
       </c>
-      <c r="F83" s="21" t="s">
-        <v>11</v>
+      <c r="F83" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="84">
@@ -1842,14 +1813,14 @@
       <c r="C84">
         <v>1</v>
       </c>
-      <c r="D84" s="17" t="s">
-        <v>7</v>
+      <c r="D84" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E84">
         <v>20.220279693603516</v>
       </c>
-      <c r="F84" s="21" t="s">
-        <v>14</v>
+      <c r="F84" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="85">
@@ -1862,14 +1833,14 @@
       <c r="C85">
         <v>0</v>
       </c>
-      <c r="D85" s="17" t="s">
+      <c r="D85" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E85">
         <v>1.36575</v>
       </c>
-      <c r="F85" s="21" t="s">
-        <v>11</v>
+      <c r="F85" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="86">
@@ -1882,14 +1853,14 @@
       <c r="C86">
         <v>0</v>
       </c>
-      <c r="D86" s="17" t="s">
+      <c r="D86" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E86">
         <v>8.7432861328125</v>
       </c>
-      <c r="F86" s="21" t="s">
-        <v>14</v>
+      <c r="F86" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="87">
@@ -1902,14 +1873,14 @@
       <c r="C87">
         <v>0</v>
       </c>
-      <c r="D87" s="17" t="s">
+      <c r="D87" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E87">
         <v>16.63175</v>
       </c>
-      <c r="F87" s="21" t="s">
-        <v>11</v>
+      <c r="F87" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="88">
@@ -1922,14 +1893,14 @@
       <c r="C88">
         <v>0</v>
       </c>
-      <c r="D88" s="17" t="s">
+      <c r="D88" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E88">
         <v>0.43645078125000641</v>
       </c>
-      <c r="F88" s="21" t="s">
-        <v>13</v>
+      <c r="F88" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="89">
@@ -1942,14 +1913,14 @@
       <c r="C89">
         <v>0</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E89">
         <v>0.5893707275390625</v>
       </c>
-      <c r="F89" s="21" t="s">
-        <v>14</v>
+      <c r="F89" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="90">
@@ -1962,14 +1933,14 @@
       <c r="C90">
         <v>0</v>
       </c>
-      <c r="D90" s="17" t="s">
+      <c r="D90" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E90">
         <v>13.468265533447266</v>
       </c>
-      <c r="F90" s="21" t="s">
-        <v>13</v>
+      <c r="F90" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="91">
@@ -1982,14 +1953,14 @@
       <c r="C91">
         <v>0</v>
       </c>
-      <c r="D91" s="17" t="s">
+      <c r="D91" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E91">
         <v>0.8697509765625</v>
       </c>
-      <c r="F91" s="21" t="s">
-        <v>13</v>
+      <c r="F91" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="92">
@@ -2002,14 +1973,14 @@
       <c r="C92">
         <v>0</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E92">
         <v>0.45919418334960938</v>
       </c>
-      <c r="F92" s="21" t="s">
-        <v>13</v>
+      <c r="F92" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="93">
@@ -2022,14 +1993,14 @@
       <c r="C93">
         <v>1</v>
       </c>
-      <c r="D93" s="17" t="s">
-        <v>10</v>
+      <c r="D93" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E93">
         <v>6.4115524291992188</v>
       </c>
-      <c r="F93" s="21" t="s">
-        <v>14</v>
+      <c r="F93" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="94">
@@ -2042,14 +2013,14 @@
       <c r="C94">
         <v>0</v>
       </c>
-      <c r="D94" s="17" t="s">
+      <c r="D94" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E94">
         <v>2.6822090148925781</v>
       </c>
-      <c r="F94" s="21" t="s">
-        <v>14</v>
+      <c r="F94" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="95">
@@ -2062,14 +2033,14 @@
       <c r="C95">
         <v>0</v>
       </c>
-      <c r="D95" s="17" t="s">
+      <c r="D95" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E95">
         <v>6.0610771179199219</v>
       </c>
-      <c r="F95" s="21" t="s">
-        <v>14</v>
+      <c r="F95" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="96">
@@ -2082,14 +2053,14 @@
       <c r="C96">
         <v>0</v>
       </c>
-      <c r="D96" s="17" t="s">
-        <v>10</v>
+      <c r="D96" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E96">
         <v>0.61082839965820313</v>
       </c>
-      <c r="F96" s="21" t="s">
-        <v>14</v>
+      <c r="F96" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="97">
@@ -2102,14 +2073,14 @@
       <c r="C97">
         <v>1</v>
       </c>
-      <c r="D97" s="17" t="s">
+      <c r="D97" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E97">
         <v>29.356956481933594</v>
       </c>
-      <c r="F97" s="21" t="s">
-        <v>14</v>
+      <c r="F97" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="98">
@@ -2122,14 +2093,14 @@
       <c r="C98">
         <v>0</v>
       </c>
-      <c r="D98" s="17" t="s">
+      <c r="D98" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E98">
         <v>1.5804181910743398</v>
       </c>
-      <c r="F98" s="21" t="s">
-        <v>12</v>
+      <c r="F98" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="99">
@@ -2142,14 +2113,14 @@
       <c r="C99">
         <v>0</v>
       </c>
-      <c r="D99" s="17" t="s">
+      <c r="D99" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E99">
         <v>0.06225461092862216</v>
       </c>
-      <c r="F99" s="21" t="s">
-        <v>12</v>
+      <c r="F99" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="100">
@@ -2162,14 +2133,14 @@
       <c r="C100">
         <v>0</v>
       </c>
-      <c r="D100" s="17" t="s">
+      <c r="D100" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E100">
         <v>5.9208869934082031</v>
       </c>
-      <c r="F100" s="21" t="s">
-        <v>14</v>
+      <c r="F100" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="101">
@@ -2182,14 +2153,14 @@
       <c r="C101">
         <v>0</v>
       </c>
-      <c r="D101" s="17" t="s">
+      <c r="D101" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E101">
         <v>1.15736981226393</v>
       </c>
-      <c r="F101" s="21" t="s">
-        <v>12</v>
+      <c r="F101" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="102">
@@ -2202,14 +2173,14 @@
       <c r="C102">
         <v>0</v>
       </c>
-      <c r="D102" s="17" t="s">
+      <c r="D102" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E102">
         <v>0.24618868867227856</v>
       </c>
-      <c r="F102" s="21" t="s">
-        <v>12</v>
+      <c r="F102" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="103">
@@ -2222,14 +2193,14 @@
       <c r="C103">
         <v>0</v>
       </c>
-      <c r="D103" s="17" t="s">
+      <c r="D103" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E103">
         <v>13.10075</v>
       </c>
-      <c r="F103" s="21" t="s">
-        <v>11</v>
+      <c r="F103" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="104">
@@ -2242,14 +2213,14 @@
       <c r="C104">
         <v>0</v>
       </c>
-      <c r="D104" s="17" t="s">
+      <c r="D104" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E104">
         <v>5.2285194396972656</v>
       </c>
-      <c r="F104" s="21" t="s">
-        <v>14</v>
+      <c r="F104" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="105">
@@ -2262,14 +2233,14 @@
       <c r="C105">
         <v>0</v>
       </c>
-      <c r="D105" s="17" t="s">
+      <c r="D105" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E105">
         <v>4.2142499999999998</v>
       </c>
-      <c r="F105" s="21" t="s">
-        <v>11</v>
+      <c r="F105" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="106">
@@ -2282,14 +2253,14 @@
       <c r="C106">
         <v>0</v>
       </c>
-      <c r="D106" s="17" t="s">
+      <c r="D106" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E106">
         <v>5.0922499999999999</v>
       </c>
-      <c r="F106" s="21" t="s">
-        <v>11</v>
+      <c r="F106" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="107">
@@ -2302,14 +2273,14 @@
       <c r="C107">
         <v>0</v>
       </c>
-      <c r="D107" s="17" t="s">
+      <c r="D107" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E107">
         <v>0.21425</v>
       </c>
-      <c r="F107" s="21" t="s">
-        <v>11</v>
+      <c r="F107" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="108">
@@ -2322,14 +2293,14 @@
       <c r="C108">
         <v>0</v>
       </c>
-      <c r="D108" s="17" t="s">
+      <c r="D108" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E108">
         <v>8.1095000000000006</v>
       </c>
-      <c r="F108" s="21" t="s">
-        <v>11</v>
+      <c r="F108" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="109">
@@ -2342,14 +2313,14 @@
       <c r="C109">
         <v>1</v>
       </c>
-      <c r="D109" s="17" t="s">
+      <c r="D109" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E109">
         <v>6.6118240356445313</v>
       </c>
-      <c r="F109" s="21" t="s">
-        <v>14</v>
+      <c r="F109" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="110">
@@ -2362,14 +2333,14 @@
       <c r="C110">
         <v>0</v>
       </c>
-      <c r="D110" s="17" t="s">
+      <c r="D110" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E110">
         <v>1.07010476232</v>
       </c>
-      <c r="F110" s="21" t="s">
-        <v>15</v>
+      <c r="F110" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="111">
@@ -2382,14 +2353,14 @@
       <c r="C111">
         <v>0</v>
       </c>
-      <c r="D111" s="17" t="s">
+      <c r="D111" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E111">
         <v>0.82985294117647057</v>
       </c>
-      <c r="F111" s="21" t="s">
-        <v>11</v>
+      <c r="F111" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="112">
@@ -2402,14 +2373,14 @@
       <c r="C112">
         <v>0</v>
       </c>
-      <c r="D112" s="17" t="s">
+      <c r="D112" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E112">
         <v>5.0902500000000002</v>
       </c>
-      <c r="F112" s="21" t="s">
-        <v>11</v>
+      <c r="F112" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="113">
@@ -2422,14 +2393,14 @@
       <c r="C113">
         <v>0</v>
       </c>
-      <c r="D113" s="17" t="s">
+      <c r="D113" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E113">
         <v>7.8384214669219716</v>
       </c>
-      <c r="F113" s="21" t="s">
-        <v>12</v>
+      <c r="F113" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="114">
@@ -2442,14 +2413,14 @@
       <c r="C114">
         <v>0</v>
       </c>
-      <c r="D114" s="17" t="s">
+      <c r="D114" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E114">
         <v>4.4092500000000001</v>
       </c>
-      <c r="F114" s="21" t="s">
-        <v>11</v>
+      <c r="F114" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="115">
@@ -2462,14 +2433,14 @@
       <c r="C115">
         <v>0</v>
       </c>
-      <c r="D115" s="17" t="s">
-        <v>7</v>
+      <c r="D115" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E115">
         <v>1.6937500000000001</v>
       </c>
-      <c r="F115" s="21" t="s">
-        <v>11</v>
+      <c r="F115" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="116">
@@ -2482,14 +2453,14 @@
       <c r="C116">
         <v>0</v>
       </c>
-      <c r="D116" s="17" t="s">
+      <c r="D116" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E116">
         <v>3.4375190734863281</v>
       </c>
-      <c r="F116" s="21" t="s">
-        <v>14</v>
+      <c r="F116" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="117">
@@ -2502,14 +2473,14 @@
       <c r="C117">
         <v>0</v>
       </c>
-      <c r="D117" s="17" t="s">
+      <c r="D117" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E117">
         <v>0.58074999999999999</v>
       </c>
-      <c r="F117" s="21" t="s">
-        <v>11</v>
+      <c r="F117" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="118">
@@ -2522,14 +2493,14 @@
       <c r="C118">
         <v>0</v>
       </c>
-      <c r="D118" s="17" t="s">
+      <c r="D118" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E118">
         <v>5.5131912231445313</v>
       </c>
-      <c r="F118" s="21" t="s">
-        <v>14</v>
+      <c r="F118" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="119">
@@ -2542,14 +2513,14 @@
       <c r="C119">
         <v>0</v>
       </c>
-      <c r="D119" s="17" t="s">
+      <c r="D119" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E119">
         <v>3.2829999999999999</v>
       </c>
-      <c r="F119" s="21" t="s">
-        <v>11</v>
+      <c r="F119" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="120">
@@ -2562,14 +2533,14 @@
       <c r="C120">
         <v>0</v>
       </c>
-      <c r="D120" s="17" t="s">
+      <c r="D120" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E120">
         <v>2.5625</v>
       </c>
-      <c r="F120" s="21" t="s">
-        <v>11</v>
+      <c r="F120" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="121">
@@ -2582,14 +2553,14 @@
       <c r="C121">
         <v>1</v>
       </c>
-      <c r="D121" s="17" t="s">
-        <v>7</v>
+      <c r="D121" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E121">
         <v>12.032999999999999</v>
       </c>
-      <c r="F121" s="21" t="s">
-        <v>13</v>
+      <c r="F121" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="122">
@@ -2602,14 +2573,14 @@
       <c r="C122">
         <v>1</v>
       </c>
-      <c r="D122" s="17" t="s">
+      <c r="D122" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E122">
         <v>3.0745288533612718</v>
       </c>
-      <c r="F122" s="21" t="s">
-        <v>12</v>
+      <c r="F122" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="123">
@@ -2622,14 +2593,14 @@
       <c r="C123">
         <v>0</v>
       </c>
-      <c r="D123" s="17" t="s">
+      <c r="D123" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E123">
         <v>2.6955</v>
       </c>
-      <c r="F123" s="21" t="s">
-        <v>13</v>
+      <c r="F123" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="124">
@@ -2642,14 +2613,14 @@
       <c r="C124">
         <v>0</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D124" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E124">
         <v>7.0361859124554078</v>
       </c>
-      <c r="F124" s="21" t="s">
-        <v>12</v>
+      <c r="F124" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>